<commit_message>
CDS Study Omic data and data mismatch issues resolved.
</commit_message>
<xml_diff>
--- a/InputFiles/CDS/TC13_CDS_Filter_Study-UCSF_Omic.xlsx
+++ b/InputFiles/CDS/TC13_CDS_Filter_Study-UCSF_Omic.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kallakuriv2\CDS Automation\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davids3\newclone\sofia0829\Commons_Automation\InputFiles\CDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2018F46D-D9D0-46A2-867D-14BE38F06098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14555DC5-D4FE-47E5-A500-3ADC41566925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -23,7 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -48,9 +53,6 @@
     <t>TabName</t>
   </si>
   <si>
-    <t>CasesTab</t>
-  </si>
-  <si>
     <t>SamplesTab</t>
   </si>
   <si>
@@ -61,32 +63,6 @@
   </si>
   <si>
     <t>TC13_CDS_Filter_Study-UCSF_Omic_WebData.xlsx</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;--(p:participant)
-OPTIONAL MATCH (p)&lt;--(samp:sample)
-OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
-OPTIONAL MATCH (samp)&lt;--(f:file)
-WITH DISTINCT samp,diag,s,p,f
-WHERE s.study_name in ["UCSF Database for the Advancement of JMML - Integration of Metadata with \"\"Omic\"\" Data"]
-RETURN
-    count(distinct s) AS Studies,
-    count(distinct p) AS Participants,
-    count(distinct samp) AS Samples,
-    count(distinct f) AS `Files`</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;--(p:participant)
-WHERE s.study_name in ["UCSF Database for the Advancement of JMML - Integration of Metadata with \"\"Omic\"\" Data"]
-OPTIONAL MATCH (p)&lt;--(samp:sample)
-WITH p, s, collect(distinct samp.sample_id) as samp
-RETURN   
- coalesce(p.participant_id,'') as `Participant ID`,
- coalesce(s.study_name, '') as `Study Name`,
- coalesce(s.phs_accession,'') as `Accession`,
- coalesce(p.gender,'') as `Gender`,
- coalesce(apoc.text.join(samp, ','), '') as `Samples`
- ORDER By p.participant_id LIMIT 100</t>
   </si>
   <si>
     <t>MATCH (s:study)&lt;--(p:participant)&lt;--(samp:sample)
@@ -102,20 +78,69 @@
 ORDER By samp.sample_id LIMIT 100</t>
   </si>
   <si>
+    <t>MATCH (s:study)
+WHERE s.study_name in ["UCSF Database for the Advancement of JMML - Integration of Metadata with \"\"Omic\"\" Data"]
+WITH s, "Not specified in data" as na
+WITH s, na, {
+    study_name: coalesce(s.study_name, na),
+    phs_accession: coalesce(s.phs_accession, na)
+} as output
+OPTIONAL MATCH (f:file)--&gt;(s)
+WITH s, na, f, apoc.map.merge(output, {
+    file_name: coalesce(f.file_name, na),
+    file_type: coalesce(f.file_type, na)
+}) as output
+WITH f, na, output
+OPTIONAL MATCH (f)--&gt;(:sample)--&gt;(p:participant)
+WITH f, na, apoc.map.merge(output, {
+    participant_id: coalesce(p.participant_id, na)
+}) as output
+OPTIONAL MATCH (f)--&gt;(samp:sample)
+WITH apoc.map.merge(output, {
+    sample_id: coalesce(samp.sample_id, na)
+}) as output
+RETURN
+    output.file_name as `File Name`,
+    output.study_name as `Study Name`,
+    output.phs_accession as `Accession`,
+    output.participant_id as `Participant ID`,
+    output.sample_id as `Sample ID`,
+    output.file_type as `File Type`
+ORDER BY `File Name` LIMIT 100</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)
+WHERE 
+    s.study_name in ["UCSF Database for the Advancement of JMML - Integration of Metadata with \"\"Omic\"\" Data"]
+WITH s, {studies: count(distinct s)} AS counts
+OPTIONAL MATCH (s)&lt;--(f:file)
+WITH s, apoc.map.merge(counts, {files: count(distinct f)}) AS counts
+OPTIONAL MATCH (s)&lt;--(p:participant)
+WITH s, apoc.map.merge(counts, {participants: count(distinct p)}) AS counts
+OPTIONAL MATCH (s)&lt;--(:participant)&lt;--(samp:sample)
+WITH apoc.map.merge(counts, {samples: count(distinct samp)}) AS counts
+RETURN
+    counts.studies AS Studies,
+    counts.participants AS Participants,
+    counts.samples AS Samples,
+    counts.files AS Files</t>
+  </si>
+  <si>
+    <t>ParticipantsTab</t>
+  </si>
+  <si>
     <t>MATCH (s:study)&lt;--(p:participant)
 WHERE s.study_name in ["UCSF Database for the Advancement of JMML - Integration of Metadata with \"\"Omic\"\" Data"]
 OPTIONAL MATCH (p)&lt;--(samp:sample)
-OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
-OPTIONAL MATCH (samp)&lt;--(f:file)
-WITH DISTINCT p,s,samp,f,diag
-RETURN 
-    coalesce(f.file_name, '') as `File Name`,
-    coalesce(s.study_name, '') as `Study Name`,
-    coalesce(s.phs_accession,'') as `Accession`,
-    coalesce(p.participant_id,'') as `Participant ID`,
-    coalesce(samp.sample_id, '') as `Sample ID`,
-    coalesce(f.file_type, '') as `File Type`
-   ORDER By f.file_name LIMIT 100</t>
+WITH s, p, apoc.coll.sort(collect(distinct coalesce(samp.sample_id, "Not specified in data"))) as samp
+RETURN   
+ coalesce(p.participant_id,'') as `Participant ID`,
+ coalesce(s.study_name, '') as `Study Name`,
+ coalesce(s.phs_accession,'') as `Accession`,
+ coalesce(p.gender,'') as `Gender`,
+ coalesce(apoc.text.join(samp, ','), '') as `Samples`
+ ORDER By p.participant_id 
+ LIMIT 100</t>
   </si>
 </sst>
 </file>
@@ -498,7 +523,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,53 +554,53 @@
     </row>
     <row r="2" spans="1:5" ht="213.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="209.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
         <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="279" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>